<commit_message>
add 33 36 37 38 covid
</commit_message>
<xml_diff>
--- a/help/27_COVID_19_svod.xlsx
+++ b/help/27_COVID_19_svod.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MedovikovOE\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharinM\Desktop\Загрузки_временные\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1947,35 +1947,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1990,25 +1965,54 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2020,10 +2024,12 @@
     <xf numFmtId="0" fontId="24" fillId="3" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2045,25 +2051,25 @@
     <xf numFmtId="0" fontId="24" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2074,12 +2080,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2755,10 +2755,10 @@
   <dimension ref="A1:AG73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="O5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="AB54" sqref="AB54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2819,72 +2819,72 @@
       <c r="AB2" s="23"/>
     </row>
     <row r="3" spans="1:28" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="181" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="189" t="s">
+      <c r="A3" s="170" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="180" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="180" t="s">
+      <c r="C3" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="183" t="s">
+      <c r="D3" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="184" t="s">
+      <c r="E3" s="173" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="170" t="s">
+      <c r="F3" s="183" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="178" t="s">
+      <c r="G3" s="188" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="179"/>
-      <c r="I3" s="179"/>
-      <c r="J3" s="179"/>
-      <c r="K3" s="179"/>
-      <c r="L3" s="179"/>
-      <c r="M3" s="179"/>
-      <c r="N3" s="179"/>
-      <c r="O3" s="179"/>
+      <c r="H3" s="189"/>
+      <c r="I3" s="189"/>
+      <c r="J3" s="189"/>
+      <c r="K3" s="189"/>
+      <c r="L3" s="189"/>
+      <c r="M3" s="189"/>
+      <c r="N3" s="189"/>
+      <c r="O3" s="189"/>
       <c r="P3" s="25"/>
-      <c r="Q3" s="187" t="s">
+      <c r="Q3" s="177" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="188" t="s">
+      <c r="R3" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="186" t="s">
+      <c r="S3" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="173"/>
-      <c r="U3" s="174" t="s">
+      <c r="T3" s="176"/>
+      <c r="U3" s="185" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="173"/>
-      <c r="W3" s="172" t="s">
+      <c r="V3" s="176"/>
+      <c r="W3" s="184" t="s">
         <v>11</v>
       </c>
-      <c r="X3" s="173"/>
-      <c r="Y3" s="177" t="s">
+      <c r="X3" s="176"/>
+      <c r="Y3" s="187" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="173"/>
-      <c r="AA3" s="175" t="s">
+      <c r="Z3" s="176"/>
+      <c r="AA3" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="AB3" s="168" t="s">
+      <c r="AB3" s="181" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="152.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="182"/>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="185"/>
-      <c r="F4" s="171"/>
+      <c r="A4" s="171"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="178"/>
       <c r="G4" s="26" t="s">
         <v>15</v>
       </c>
@@ -2915,8 +2915,8 @@
       <c r="P4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="Q4" s="171"/>
-      <c r="R4" s="176"/>
+      <c r="Q4" s="178"/>
+      <c r="R4" s="169"/>
       <c r="S4" s="27" t="s">
         <v>25</v>
       </c>
@@ -2941,8 +2941,8 @@
       <c r="Z4" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AA4" s="176"/>
-      <c r="AB4" s="169"/>
+      <c r="AA4" s="169"/>
+      <c r="AB4" s="182"/>
     </row>
     <row r="5" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
@@ -3588,11 +3588,11 @@
         <v>#N/A</v>
       </c>
       <c r="AA10" s="83" t="e">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(AA11:AA37)</f>
         <v>#N/A</v>
       </c>
       <c r="AB10" s="83" t="e">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(AB11:AB37)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -6723,11 +6723,11 @@
         <v>#N/A</v>
       </c>
       <c r="AA38" s="152" t="e">
-        <f>SUM(AA39:AA52)</f>
+        <f>AVERAGE(AA39:AA52)</f>
         <v>#N/A</v>
       </c>
       <c r="AB38" s="152" t="e">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AB39:AB52)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8310,7 +8310,7 @@
         <v>#N/A</v>
       </c>
       <c r="E53" s="151" t="e">
-        <f t="shared" ref="E53:AB53" si="5">SUM(E54:E73)</f>
+        <f t="shared" ref="E53:AA53" si="5">SUM(E54:E73)</f>
         <v>#N/A</v>
       </c>
       <c r="F53" s="151" t="e">
@@ -8398,11 +8398,11 @@
         <v>#N/A</v>
       </c>
       <c r="AA53" s="151" t="e">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(AA54:AA73)</f>
         <v>#N/A</v>
       </c>
       <c r="AB53" s="151" t="e">
-        <f>SUM(AB54:AB73)</f>
+        <f>AVERAGE(AB54:AB73)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -10648,6 +10648,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="G3:O3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="D3:D4"/>
@@ -10656,13 +10663,6 @@
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="G3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="10" fitToHeight="0" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -10695,107 +10695,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="206" t="s">
+      <c r="B1" s="190" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="208" t="s">
+      <c r="C1" s="193" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="209" t="s">
+      <c r="D1" s="194" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="210" t="s">
+      <c r="E1" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="197" t="s">
+      <c r="F1" s="200" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
-      <c r="P1" s="199" t="s">
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
+      <c r="M1" s="191"/>
+      <c r="N1" s="191"/>
+      <c r="O1" s="191"/>
+      <c r="P1" s="201" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="199" t="s">
+      <c r="Q1" s="201" t="s">
         <v>110</v>
       </c>
-      <c r="R1" s="199" t="s">
+      <c r="R1" s="201" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="198"/>
-      <c r="T1" s="201" t="s">
+      <c r="S1" s="191"/>
+      <c r="T1" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="198"/>
-      <c r="V1" s="202" t="s">
+      <c r="U1" s="191"/>
+      <c r="V1" s="204" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="198"/>
-      <c r="X1" s="203" t="s">
+      <c r="W1" s="191"/>
+      <c r="X1" s="205" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="198"/>
-      <c r="Z1" s="200" t="s">
+      <c r="Y1" s="191"/>
+      <c r="Z1" s="202" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="200" t="s">
+      <c r="AA1" s="202" t="s">
         <v>93</v>
       </c>
-      <c r="AB1" s="205" t="s">
+      <c r="AB1" s="207" t="s">
         <v>108</v>
       </c>
-      <c r="AC1" s="194" t="s">
+      <c r="AC1" s="196" t="s">
         <v>105</v>
       </c>
       <c r="AD1" s="155" t="s">
         <v>106</v>
       </c>
-      <c r="AE1" s="204"/>
-      <c r="AF1" s="195" t="s">
+      <c r="AE1" s="206"/>
+      <c r="AF1" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="196" t="s">
+      <c r="AG1" s="198" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="190" t="s">
+      <c r="AH1" s="208" t="s">
         <v>5</v>
       </c>
-      <c r="AI1" s="192" t="s">
+      <c r="AI1" s="209" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="192" t="s">
+      <c r="AJ1" s="209" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="192" t="s">
+      <c r="AK1" s="209" t="s">
         <v>90</v>
       </c>
-      <c r="AL1" s="191"/>
+      <c r="AL1" s="199"/>
       <c r="AM1" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="193" t="s">
+      <c r="AN1" s="210" t="s">
         <v>11</v>
       </c>
-      <c r="AO1" s="191"/>
+      <c r="AO1" s="199"/>
       <c r="AP1" s="126" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:42" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="198"/>
-      <c r="B2" s="198"/>
-      <c r="C2" s="208"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
+      <c r="A2" s="191"/>
+      <c r="B2" s="191"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
       <c r="F2" s="100" t="s">
         <v>15</v>
       </c>
@@ -10826,8 +10826,8 @@
       <c r="O2" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="198"/>
-      <c r="Q2" s="198"/>
+      <c r="P2" s="191"/>
+      <c r="Q2" s="191"/>
       <c r="R2" s="101" t="s">
         <v>25</v>
       </c>
@@ -10852,19 +10852,19 @@
       <c r="Y2" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="198"/>
-      <c r="AA2" s="198"/>
-      <c r="AB2" s="205"/>
-      <c r="AC2" s="194"/>
+      <c r="Z2" s="191"/>
+      <c r="AA2" s="191"/>
+      <c r="AB2" s="207"/>
+      <c r="AC2" s="196"/>
       <c r="AD2" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="AE2" s="204"/>
-      <c r="AF2" s="195"/>
-      <c r="AG2" s="191"/>
-      <c r="AH2" s="191"/>
-      <c r="AI2" s="191"/>
-      <c r="AJ2" s="191"/>
+      <c r="AE2" s="206"/>
+      <c r="AF2" s="197"/>
+      <c r="AG2" s="199"/>
+      <c r="AH2" s="199"/>
+      <c r="AI2" s="199"/>
+      <c r="AJ2" s="199"/>
       <c r="AK2" s="118" t="s">
         <v>25</v>
       </c>
@@ -10998,7 +10998,7 @@
         <f>W3-Y3</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="204"/>
+      <c r="AE3" s="206"/>
       <c r="AF3" s="127">
         <f>IF(C3&gt;=U3,0,1)</f>
         <v>0</v>
@@ -18801,11 +18801,11 @@
   </sheetData>
   <autoFilter ref="A3:AB43"/>
   <mergeCells count="24">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AG1:AG2"/>
@@ -18820,11 +18820,11 @@
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AE1:AE3"/>
     <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="cellIs" dxfId="43" priority="44" operator="lessThan">
@@ -19820,68 +19820,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="217" t="s">
+      <c r="B1" s="212" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="218" t="s">
+      <c r="C1" s="213" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="209" t="s">
+      <c r="D1" s="194" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="210" t="s">
+      <c r="E1" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="210" t="s">
+      <c r="F1" s="195" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="212"/>
-      <c r="H1" s="212"/>
-      <c r="I1" s="212"/>
-      <c r="J1" s="212"/>
-      <c r="K1" s="212"/>
-      <c r="L1" s="212"/>
-      <c r="M1" s="212"/>
-      <c r="N1" s="212"/>
-      <c r="O1" s="212"/>
-      <c r="P1" s="213" t="s">
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="211"/>
+      <c r="L1" s="211"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="211"/>
+      <c r="O1" s="211"/>
+      <c r="P1" s="215" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="213" t="s">
+      <c r="Q1" s="215" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="213" t="s">
+      <c r="R1" s="215" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="212"/>
-      <c r="T1" s="214" t="s">
+      <c r="S1" s="211"/>
+      <c r="T1" s="216" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="212"/>
-      <c r="V1" s="215" t="s">
+      <c r="U1" s="211"/>
+      <c r="V1" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="212"/>
-      <c r="X1" s="216" t="s">
+      <c r="W1" s="211"/>
+      <c r="X1" s="218" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="212"/>
-      <c r="Z1" s="211" t="s">
+      <c r="Y1" s="211"/>
+      <c r="Z1" s="214" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="211" t="s">
+      <c r="AA1" s="214" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="220.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="212"/>
-      <c r="B2" s="212"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
+      <c r="A2" s="211"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="213"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
       <c r="F2" s="130" t="s">
         <v>15</v>
       </c>
@@ -19912,8 +19912,8 @@
       <c r="O2" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="212"/>
-      <c r="Q2" s="212"/>
+      <c r="P2" s="211"/>
+      <c r="Q2" s="211"/>
       <c r="R2" s="131" t="s">
         <v>25</v>
       </c>
@@ -19938,8 +19938,8 @@
       <c r="Y2" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="212"/>
-      <c r="AA2" s="212"/>
+      <c r="Z2" s="211"/>
+      <c r="AA2" s="211"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="134" t="s">
@@ -22862,12 +22862,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F1:O1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="P1:P2"/>
@@ -22876,6 +22870,12 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="F1:O1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E100">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">

</xml_diff>